<commit_message>
Amelioration affichage des tableaux
</commit_message>
<xml_diff>
--- a/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
+++ b/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="domaine" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="categorie" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="indicateur" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="type indicateur" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$C$27</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="247">
   <si>
     <t xml:space="preserve">idDomaine</t>
   </si>
@@ -582,6 +583,252 @@
   </si>
   <si>
     <t xml:space="preserve">Absence du tout à l’égout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">typeIndicateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelTypeIndicateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effectifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effectifs pondérés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part_np</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part non pondérée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part (en%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq.ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq.pauv60.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individus sous le seuil à 60 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq.pauv50.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individus sous le seuil à 50 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq.pauv40.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individus sous le seuil à 40 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx_pauv60.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taux de pauvreté à 60 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx_pauv50.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taux de pauvreté à 50 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx_pauv40.ind.metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taux de pauvreté à 40 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre d’individus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moyenne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantile 1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantile 5 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">er</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> décile</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2ème décile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.25</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">er</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> quartile</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médiane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3ème quartile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ème décile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9ème décile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantile 95 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantile 99 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d9_d1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecart D9/D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q4_q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecart D8/D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d5_d1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecart D5/D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d9_d5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecart D9/D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">superficie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superficie (en m²)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">densitepop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Densité de population (en hab / km²)</t>
   </si>
 </sst>
 </file>
@@ -591,7 +838,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -613,6 +860,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -657,13 +912,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1195,8 +1454,8 @@
   </sheetPr>
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P56" activeCellId="0" sqref="P56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2476,4 +2735,289 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Amélioration du calcul statistique et de l'affichage
</commit_message>
<xml_diff>
--- a/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
+++ b/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
@@ -12,11 +12,12 @@
     <sheet name="categorie" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="indicateur" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="type indicateur" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Zone predefinie" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$C$27</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$27</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$D$74</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$C$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="257">
   <si>
     <t xml:space="preserve">idDomaine</t>
   </si>
@@ -822,13 +823,43 @@
     <t xml:space="preserve">superficie</t>
   </si>
   <si>
-    <t xml:space="preserve">Superficie (en m²)</t>
+    <t xml:space="preserve">Superficie (en km²)</t>
   </si>
   <si>
     <t xml:space="preserve">densitepop</t>
   </si>
   <si>
     <t xml:space="preserve">Densité de population (en hab / km²)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idZonage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant de la zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idZonage.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idPredefine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelPredefine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Département</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonage utilisateur</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1466,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C27"/>
+  <autoFilter ref="A1:D27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2742,10 +2773,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3002,8 +3033,22 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3020,4 +3065,71 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout du secret statistique
</commit_message>
<xml_diff>
--- a/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
+++ b/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="domaine" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,10 +15,10 @@
     <sheet name="Zone predefinie" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$27</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$F$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$C$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$C$27</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$D$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$F$75</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="324">
   <si>
     <t xml:space="preserve">idDomaine</t>
   </si>
@@ -1014,6 +1014,36 @@
   </si>
   <si>
     <t xml:space="preserve">Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret_stat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret statistique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoefVariation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficient de variation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EstVariable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur estimée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IntervalConf.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalle de confiance à 95 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur diffusée dans le tableau de bord</t>
   </si>
   <si>
     <t xml:space="preserve">idPredefine</t>
@@ -1638,7 +1668,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D27"/>
+  <autoFilter ref="A1:C27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1657,7 +1687,7 @@
   </sheetPr>
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -3097,7 +3127,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F75"/>
+  <autoFilter ref="A1:D75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3114,10 +3144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3390,11 +3420,46 @@
         <v>307</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3426,10 +3491,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3437,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,7 +3510,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,7 +3518,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3526,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>